<commit_message>
Modify RGAA pre-audit checklist: added sampling tab
</commit_message>
<xml_diff>
--- a/.storybook/public/documents/Checklist_pre-audit_CNAM_NOM_DU_PRODUIT.xlsx
+++ b/.storybook/public/documents/Checklist_pre-audit_CNAM_NOM_DU_PRODUIT.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/julien_roche_fabernovel_ey_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien.Roche/code/cnam/design-system-v3/.storybook/public/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="8_{1BA491FE-60BE-0942-B63C-E8C80F25D501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78858204-3CCC-EC4A-8B85-92C94501DA32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DB499A-CB48-E342-BBFA-03D4AE5734A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17680" activeTab="1" xr2:uid="{352E66E6-3C64-8D43-8BDA-4113AEA1A882}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{352E66E6-3C64-8D43-8BDA-4113AEA1A882}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations" sheetId="2" r:id="rId1"/>
-    <sheet name="Pré-audit - Template" sheetId="1" r:id="rId2"/>
+    <sheet name="Échantillonnage" sheetId="3" r:id="rId2"/>
+    <sheet name="Pré-audit - Template" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Tableau_Fonctionnalités">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Critère</t>
   </si>
@@ -91,9 +95,6 @@
   </si>
   <si>
     <t>URL de la page (si site web)</t>
-  </si>
-  <si>
-    <t>Échantillon *</t>
   </si>
   <si>
     <t>Nom de la page *</t>
@@ -131,6 +132,235 @@
   </si>
   <si>
     <t>Vérification manuelle :</t>
+  </si>
+  <si>
+    <t>Nom de la page</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Accueil</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Mention légales</t>
+  </si>
+  <si>
+    <t>Plan du site</t>
+  </si>
+  <si>
+    <t>Aide</t>
+  </si>
+  <si>
+    <t>Authentification</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Date de l'échantillonnage</t>
+  </si>
+  <si>
+    <t>Échantillonnage</t>
+  </si>
+  <si>
+    <t>Typologie de page obligatoire RGAA</t>
+  </si>
+  <si>
+    <t>Au moins 1 page pertinente pour chaque type de service fourni (ex: rubriques de 1er niveau), y compris la fonctionnalité de recherche et ses pages de résultat</t>
+  </si>
+  <si>
+    <t>Au moins 1 document téléchargeable pertinent</t>
+  </si>
+  <si>
+    <t>Ensemble des pages constituant un processus (ex: un formulaire sur plusieurs pages)</t>
+  </si>
+  <si>
+    <t>Pages sélectionnées au hasard représentant à minima 10% de l’échantillon</t>
+  </si>
+  <si>
+    <t>Exemples de pages ayant un aspect sensiblement distinct ou présentation un type de contenu différent (ex : page contenant des tableaux de données, des éléments multimédias, des illustrations, des formulaires, etc.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pensez à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>scroller horizontalement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour accéder à l'ensemble du contenu et du tableau.
+Le RGAA exige que l’audit d’accessibilité soit effectué sur un ensemble représentatif de pages et des fonctionnalités de votre service. Il serait difficile et très chronophage de tester l’intégralité des contenus. La définition d’un périmètre est un compromis pertinent pour auditer efficacement un service et respecter les exigences légales.
+L'échantillonnage est la selection des pages concernées par le pré-audit et l'audit d'accessibilité. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Utilisez le tableau dans la partie "Échantillonage" (ligne 9)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour lister l'ensemble des pages du produit au regard des exigences du RGAA indiquées dans la colonne "Typologie de page obligatoire RGAA".</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Échantillonnage :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">L'objectif est de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>lister les pages du produit à sélectionner en fonction des typologies de pages requises pour un audit RGAA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+Vous pouvez </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>supprimer les lignes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> correspondant à des typologies pour lesquelles vous </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ne disposez d’aucune page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. À l’inverse, vous pouvez </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>dupliquer les lignes pour ajouter plusieurs pages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> relevant d’une même typologie si cela est nécessaire.
+Chaque page retenue doit avoir un onglet dédié. Créez une copie de l'onglet "Pré-audit - Template" et renommez-le pour chaque page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note sur les contenus exemptés :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Certains contenus sont exemptés de l’obligation d’accessibilité et se situent hors champ de l’obligation légale :
+1- Les fichiers disponibles dans des formats bureautiques publiés avant le 23 septembre 2018, sauf s’ils sont nécessaires à l’accomplissement d’une démarche administrative relevant des tâches effectuées par l’organisme concerné ;
+2- Les contenus audio et vidéo préenregistrés, y compris ceux comprenant des composants interactifs, publiés avant le 23 septembre 2020 ;
+3- Les contenus audio et vidéo diffusés en direct, y compris ceux comprenant des composants interactifs ;
+4- Les cartes et les services de cartographie en ligne, sous réserve que, s’agissant des cartes destinées à fournir une localisation ou un itinéraire, les informations essentielles soient fournies sous une forme numérique accessible ;
+5- Les contenus de tiers qui ne sont ni financés ni développés par l’organisme concerné et qui ne sont pas sous son contrôle ;
+6- Les reproductions de pièces de collections patrimoniales qui ne peuvent être rendues totalement accessibles en raison :
+    - Soit de l’incompatibilité des exigences en matière d’accessibilité avec la préservation de la pièce concernée ou l’authenticité de la reproduction notamment en termes de contraste ;
+    - Soit de l’indisponibilité de solutions automatisées et économiques qui permettraient de transcrire facilement le texte de manuscrits ou d’autres pièces de collections patrimoniales et de le restituer sous la forme d’un contenu compatible avec l’obligation d’accessibilité ;
+7- Les contenus des intranets et des extranets publiés avant le 23 septembre 2019, jusqu’à ce que ces sites fassent l’objet d’une révision en profondeur ;
+8- Les contenus des sites internet et des applications mobiles qui ne sont ni nécessaires à l’accomplissement d’une démarche administrative active ni mis à jour ou modifiés après le 23 septembre 2019, notamment les archives.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -146,42 +376,42 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <u/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="18"/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow (Corps)"/>
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,12 +436,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7ECF5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -336,70 +560,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -451,11 +703,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -464,7 +716,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -472,118 +724,6 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -600,11 +740,129 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="0"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -623,13 +881,222 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000091"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF000091"/>
       <color rgb="FFE7ECF5"/>
       <color rgb="FFF0F0F0"/>
-      <color rgb="FF000091"/>
     </mruColors>
   </colors>
   <extLst>
@@ -644,7 +1111,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5818454-E70D-B94A-A148-9A3DA5386362}" name="Critère_préaudit_manuel_page1" displayName="Critère_préaudit_manuel_page1" ref="A11:C19" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{01C3A2C5-A429-F947-B00E-62C2EA075D12}" name="Tableau4" displayName="Tableau4" ref="A13:D25" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A13:D25" xr:uid="{01C3A2C5-A429-F947-B00E-62C2EA075D12}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3AD2848C-780A-AE4F-8C53-3AF4A443BB58}" name="Typologie de page obligatoire RGAA" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E2C7F0E0-A6CE-3341-95E3-D5D4EDA09CD4}" name="Nom de la page" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F208A1C8-7A3E-C94D-B28D-F4100CAC9FB1}" name="URL" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{51852F65-B03F-FA43-B150-1B177E21B0EC}" name="Commentaire" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5818454-E70D-B94A-A148-9A3DA5386362}" name="Critère_préaudit_manuel_page1" displayName="Critère_préaudit_manuel_page1" ref="A11:C19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A11:C19" xr:uid="{E5818454-E70D-B94A-A148-9A3DA5386362}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BD3D3CC7-B942-AA4B-82D8-8A73E00D7D09}" name="Critère" dataDxfId="6"/>
@@ -972,10 +1452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8550ED5-89BC-2846-B3BC-5EDDF05F9AC9}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,78 +1465,77 @@
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-    </row>
-    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="30"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="16"/>
-    </row>
-    <row r="5" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" ht="205" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" ht="209" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" ht="224" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1078,18 +1557,16 @@
     <row r="32" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il est important de faire le pré-audit sur une même version du votre produit. Indiquez le numéro (ou le nom) de la version en question." sqref="B7" xr:uid="{AE50BA18-C4AD-FC40-9A60-EC7997756DEE}">
       <formula1>"Site web &amp; mobile,Site web uniquement,Application mobile,Client lourd"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lister les pages de l'échantillon de test à auditer._x000a_Dupliquer l'onglet &quot;Pré-audit - Template&quot; pour chaque page._x000a_Voir documentation rubrique &quot;Kit de pré-audit&quot;" sqref="B12" xr:uid="{7B15E808-8545-DE45-894C-A0C790CE6B45}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="N'hésitez pas à ajouter des informations complémentaires ou vos questions. Nous sommes là pour vous aider." sqref="B13" xr:uid="{E53FE9A2-AB32-CC4C-B8EE-62512D3F5290}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="N'hésitez pas à ajouter des informations complémentaires ou vos questions. Nous sommes là pour vous aider." sqref="B12" xr:uid="{E53FE9A2-AB32-CC4C-B8EE-62512D3F5290}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="- Site web : accessible sur navigateur ordinateur (et mobile ?)_x000a_- Application mobile native : spécifique à une plateforme mobile (iOS/Android)_x000a_- Client lourd : logiciel installé localement sur un ordinateur" sqref="B6" xr:uid="{895BD7CA-69D9-B543-AD56-148F64D59B5C}">
       <formula1>"Site web (ordinateur et mobile),Site web (ordinateur uniquement),Application mobile,Client lourd"</formula1>
     </dataValidation>
@@ -1100,11 +1577,248 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2089FE98-4A7F-4947-9D3A-B2FAE1C7AAD3}">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="68" style="1" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="271" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+    </row>
+    <row r="7" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Format JJ/MM/AAAA" sqref="B11" xr:uid="{73F963BB-9FDA-DF40-A22A-85FA3BE3B4E1}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BC96EE-2721-B644-B048-A1FEC470793D}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,146 +1829,169 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="str">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="str">
         <f>"Pré-audit de la page """ &amp; B5  &amp; """"</f>
         <v>Pré-audit de la page "Template"</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="3" spans="1:3" ht="77" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="34"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="34"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="18"/>
-    </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-    </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-    </row>
-    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="21" spans="1:3" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="171" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1280,11 +2017,10 @@
       <formula>$B12="Non conforme"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B19" xr:uid="{D14CA0B8-36C3-754A-9C76-46313372ABD3}">
       <formula1>"Conforme,Non conforme,Non applicable,Dérogé,Non testé"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Format JJ/MM/AAAA" sqref="B6:C6" xr:uid="{CDF212B3-9E48-7A44-A15F-DEAA76FB8C67}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="N'hésitez pas à ajouter des informations complémentaires ou vos questions. Nous sommes là pour vous aider." sqref="B21:C21" xr:uid="{F5327884-B679-904A-8B76-54E006C3FE12}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify RGAA pre-audit checklist: added sampling tab (#562)
Co-authored-by: Julien Roche <6241568+JulienRoche@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/.storybook/public/documents/Checklist_pre-audit_CNAM_NOM_DU_PRODUIT.xlsx
+++ b/.storybook/public/documents/Checklist_pre-audit_CNAM_NOM_DU_PRODUIT.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/julien_roche_fabernovel_ey_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien.Roche/code/cnam/design-system-v3/.storybook/public/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="8_{1BA491FE-60BE-0942-B63C-E8C80F25D501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78858204-3CCC-EC4A-8B85-92C94501DA32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DB499A-CB48-E342-BBFA-03D4AE5734A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17680" activeTab="1" xr2:uid="{352E66E6-3C64-8D43-8BDA-4113AEA1A882}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{352E66E6-3C64-8D43-8BDA-4113AEA1A882}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations" sheetId="2" r:id="rId1"/>
-    <sheet name="Pré-audit - Template" sheetId="1" r:id="rId2"/>
+    <sheet name="Échantillonnage" sheetId="3" r:id="rId2"/>
+    <sheet name="Pré-audit - Template" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Tableau_Fonctionnalités">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Critère</t>
   </si>
@@ -91,9 +95,6 @@
   </si>
   <si>
     <t>URL de la page (si site web)</t>
-  </si>
-  <si>
-    <t>Échantillon *</t>
   </si>
   <si>
     <t>Nom de la page *</t>
@@ -131,6 +132,235 @@
   </si>
   <si>
     <t>Vérification manuelle :</t>
+  </si>
+  <si>
+    <t>Nom de la page</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Accueil</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Mention légales</t>
+  </si>
+  <si>
+    <t>Plan du site</t>
+  </si>
+  <si>
+    <t>Aide</t>
+  </si>
+  <si>
+    <t>Authentification</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Date de l'échantillonnage</t>
+  </si>
+  <si>
+    <t>Échantillonnage</t>
+  </si>
+  <si>
+    <t>Typologie de page obligatoire RGAA</t>
+  </si>
+  <si>
+    <t>Au moins 1 page pertinente pour chaque type de service fourni (ex: rubriques de 1er niveau), y compris la fonctionnalité de recherche et ses pages de résultat</t>
+  </si>
+  <si>
+    <t>Au moins 1 document téléchargeable pertinent</t>
+  </si>
+  <si>
+    <t>Ensemble des pages constituant un processus (ex: un formulaire sur plusieurs pages)</t>
+  </si>
+  <si>
+    <t>Pages sélectionnées au hasard représentant à minima 10% de l’échantillon</t>
+  </si>
+  <si>
+    <t>Exemples de pages ayant un aspect sensiblement distinct ou présentation un type de contenu différent (ex : page contenant des tableaux de données, des éléments multimédias, des illustrations, des formulaires, etc.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pensez à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>scroller horizontalement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour accéder à l'ensemble du contenu et du tableau.
+Le RGAA exige que l’audit d’accessibilité soit effectué sur un ensemble représentatif de pages et des fonctionnalités de votre service. Il serait difficile et très chronophage de tester l’intégralité des contenus. La définition d’un périmètre est un compromis pertinent pour auditer efficacement un service et respecter les exigences légales.
+L'échantillonnage est la selection des pages concernées par le pré-audit et l'audit d'accessibilité. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Utilisez le tableau dans la partie "Échantillonage" (ligne 9)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour lister l'ensemble des pages du produit au regard des exigences du RGAA indiquées dans la colonne "Typologie de page obligatoire RGAA".</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Échantillonnage :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">L'objectif est de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>lister les pages du produit à sélectionner en fonction des typologies de pages requises pour un audit RGAA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+Vous pouvez </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>supprimer les lignes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> correspondant à des typologies pour lesquelles vous </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ne disposez d’aucune page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. À l’inverse, vous pouvez </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>dupliquer les lignes pour ajouter plusieurs pages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> relevant d’une même typologie si cela est nécessaire.
+Chaque page retenue doit avoir un onglet dédié. Créez une copie de l'onglet "Pré-audit - Template" et renommez-le pour chaque page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note sur les contenus exemptés :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Certains contenus sont exemptés de l’obligation d’accessibilité et se situent hors champ de l’obligation légale :
+1- Les fichiers disponibles dans des formats bureautiques publiés avant le 23 septembre 2018, sauf s’ils sont nécessaires à l’accomplissement d’une démarche administrative relevant des tâches effectuées par l’organisme concerné ;
+2- Les contenus audio et vidéo préenregistrés, y compris ceux comprenant des composants interactifs, publiés avant le 23 septembre 2020 ;
+3- Les contenus audio et vidéo diffusés en direct, y compris ceux comprenant des composants interactifs ;
+4- Les cartes et les services de cartographie en ligne, sous réserve que, s’agissant des cartes destinées à fournir une localisation ou un itinéraire, les informations essentielles soient fournies sous une forme numérique accessible ;
+5- Les contenus de tiers qui ne sont ni financés ni développés par l’organisme concerné et qui ne sont pas sous son contrôle ;
+6- Les reproductions de pièces de collections patrimoniales qui ne peuvent être rendues totalement accessibles en raison :
+    - Soit de l’incompatibilité des exigences en matière d’accessibilité avec la préservation de la pièce concernée ou l’authenticité de la reproduction notamment en termes de contraste ;
+    - Soit de l’indisponibilité de solutions automatisées et économiques qui permettraient de transcrire facilement le texte de manuscrits ou d’autres pièces de collections patrimoniales et de le restituer sous la forme d’un contenu compatible avec l’obligation d’accessibilité ;
+7- Les contenus des intranets et des extranets publiés avant le 23 septembre 2019, jusqu’à ce que ces sites fassent l’objet d’une révision en profondeur ;
+8- Les contenus des sites internet et des applications mobiles qui ne sont ni nécessaires à l’accomplissement d’une démarche administrative active ni mis à jour ou modifiés après le 23 septembre 2019, notamment les archives.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -146,42 +376,42 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <u/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="18"/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow (Corps)"/>
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,12 +436,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7ECF5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -336,70 +560,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -451,11 +703,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -464,7 +716,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -472,118 +724,6 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -600,11 +740,129 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="0"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -623,13 +881,222 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000091"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF000091"/>
       <color rgb="FFE7ECF5"/>
       <color rgb="FFF0F0F0"/>
-      <color rgb="FF000091"/>
     </mruColors>
   </colors>
   <extLst>
@@ -644,7 +1111,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5818454-E70D-B94A-A148-9A3DA5386362}" name="Critère_préaudit_manuel_page1" displayName="Critère_préaudit_manuel_page1" ref="A11:C19" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{01C3A2C5-A429-F947-B00E-62C2EA075D12}" name="Tableau4" displayName="Tableau4" ref="A13:D25" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A13:D25" xr:uid="{01C3A2C5-A429-F947-B00E-62C2EA075D12}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3AD2848C-780A-AE4F-8C53-3AF4A443BB58}" name="Typologie de page obligatoire RGAA" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E2C7F0E0-A6CE-3341-95E3-D5D4EDA09CD4}" name="Nom de la page" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F208A1C8-7A3E-C94D-B28D-F4100CAC9FB1}" name="URL" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{51852F65-B03F-FA43-B150-1B177E21B0EC}" name="Commentaire" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5818454-E70D-B94A-A148-9A3DA5386362}" name="Critère_préaudit_manuel_page1" displayName="Critère_préaudit_manuel_page1" ref="A11:C19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A11:C19" xr:uid="{E5818454-E70D-B94A-A148-9A3DA5386362}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BD3D3CC7-B942-AA4B-82D8-8A73E00D7D09}" name="Critère" dataDxfId="6"/>
@@ -972,10 +1452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8550ED5-89BC-2846-B3BC-5EDDF05F9AC9}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,78 +1465,77 @@
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-    </row>
-    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="30"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="16"/>
-    </row>
-    <row r="5" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" ht="205" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" ht="209" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" ht="224" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1078,18 +1557,16 @@
     <row r="32" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il est important de faire le pré-audit sur une même version du votre produit. Indiquez le numéro (ou le nom) de la version en question." sqref="B7" xr:uid="{AE50BA18-C4AD-FC40-9A60-EC7997756DEE}">
       <formula1>"Site web &amp; mobile,Site web uniquement,Application mobile,Client lourd"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lister les pages de l'échantillon de test à auditer._x000a_Dupliquer l'onglet &quot;Pré-audit - Template&quot; pour chaque page._x000a_Voir documentation rubrique &quot;Kit de pré-audit&quot;" sqref="B12" xr:uid="{7B15E808-8545-DE45-894C-A0C790CE6B45}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="N'hésitez pas à ajouter des informations complémentaires ou vos questions. Nous sommes là pour vous aider." sqref="B13" xr:uid="{E53FE9A2-AB32-CC4C-B8EE-62512D3F5290}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="N'hésitez pas à ajouter des informations complémentaires ou vos questions. Nous sommes là pour vous aider." sqref="B12" xr:uid="{E53FE9A2-AB32-CC4C-B8EE-62512D3F5290}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="- Site web : accessible sur navigateur ordinateur (et mobile ?)_x000a_- Application mobile native : spécifique à une plateforme mobile (iOS/Android)_x000a_- Client lourd : logiciel installé localement sur un ordinateur" sqref="B6" xr:uid="{895BD7CA-69D9-B543-AD56-148F64D59B5C}">
       <formula1>"Site web (ordinateur et mobile),Site web (ordinateur uniquement),Application mobile,Client lourd"</formula1>
     </dataValidation>
@@ -1100,11 +1577,248 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2089FE98-4A7F-4947-9D3A-B2FAE1C7AAD3}">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="68" style="1" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="271" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+    </row>
+    <row r="7" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Format JJ/MM/AAAA" sqref="B11" xr:uid="{73F963BB-9FDA-DF40-A22A-85FA3BE3B4E1}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BC96EE-2721-B644-B048-A1FEC470793D}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,146 +1829,169 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="str">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="str">
         <f>"Pré-audit de la page """ &amp; B5  &amp; """"</f>
         <v>Pré-audit de la page "Template"</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="3" spans="1:3" ht="77" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="34"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="34"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="18"/>
-    </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-    </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-    </row>
-    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="21" spans="1:3" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="171" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1280,11 +2017,10 @@
       <formula>$B12="Non conforme"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B19" xr:uid="{D14CA0B8-36C3-754A-9C76-46313372ABD3}">
       <formula1>"Conforme,Non conforme,Non applicable,Dérogé,Non testé"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Format JJ/MM/AAAA" sqref="B6:C6" xr:uid="{CDF212B3-9E48-7A44-A15F-DEAA76FB8C67}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="N'hésitez pas à ajouter des informations complémentaires ou vos questions. Nous sommes là pour vous aider." sqref="B21:C21" xr:uid="{F5327884-B679-904A-8B76-54E006C3FE12}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>